<commit_message>
updated supplementary tables, include PERMANOVA results
</commit_message>
<xml_diff>
--- a/data/comm.rates/Supplementary_Tables.xlsx
+++ b/data/comm.rates/Supplementary_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angelrain/Documents/Github/chemo.disturbances/chemo.disturbances/data/comm.rates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37EFFF1-E615-C942-BDF3-BA08C4300CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B89958A-46B1-EE4D-8DF0-ACCB61C62F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="500" windowWidth="12120" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16180" yWindow="500" windowWidth="12620" windowHeight="15800" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="16" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4388" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4389" uniqueCount="220">
   <si>
     <t>Date</t>
   </si>
@@ -876,6 +876,9 @@
   <si>
     <t>DOM level:Disturbance regime</t>
   </si>
+  <si>
+    <t>.</t>
+  </si>
 </sst>
 </file>
 
@@ -884,7 +887,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -962,6 +965,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -977,7 +986,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1000,11 +1009,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1076,19 +1122,25 @@
     <xf numFmtId="11" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1405,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB10CD6-6E1D-774C-B88A-61E7784C66BF}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="C11:D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1419,15 +1471,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="B1" s="37" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="9" t="s">
         <v>214</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1441,115 +1492,112 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="34" t="s">
         <v>216</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C3" s="35">
-        <v>22.477</v>
-      </c>
-      <c r="D3" s="36">
+      <c r="C3" s="32">
+        <v>30.0928</v>
+      </c>
+      <c r="D3" s="33">
         <v>9.990000000000001E-4</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F3" s="33"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C4" s="35">
-        <v>2.4796999999999998</v>
-      </c>
-      <c r="D4" s="36">
-        <v>2.997E-2</v>
+      <c r="C4" s="32">
+        <v>3.3334000000000001</v>
+      </c>
+      <c r="D4" s="33">
+        <v>7.9920000000000008E-3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F4" s="33"/>
+        <v>209</v>
+      </c>
+      <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="C5" s="35">
-        <v>52.287599999999998</v>
-      </c>
-      <c r="D5" s="36">
+      <c r="C5" s="32">
+        <v>14.2272</v>
+      </c>
+      <c r="D5" s="33">
         <v>9.990000000000001E-4</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="C6" s="35">
-        <v>2.8014000000000001</v>
-      </c>
-      <c r="D6" s="36">
-        <v>1.0989000000000001E-2</v>
+      <c r="C6" s="32">
+        <v>3.7523</v>
+      </c>
+      <c r="D6" s="33">
+        <v>2.9970000000000001E-3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F6" s="33"/>
+        <v>209</v>
+      </c>
+      <c r="F6" s="31"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="C7" s="35">
-        <v>2.8488000000000002</v>
-      </c>
-      <c r="D7" s="36">
-        <v>1.6983000000000002E-2</v>
+      <c r="C7" s="32">
+        <v>2.2831000000000001</v>
+      </c>
+      <c r="D7" s="33">
+        <v>9.990000000000001E-4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F7" s="33"/>
+        <v>203</v>
+      </c>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="C8" s="35">
-        <v>0.7399</v>
-      </c>
-      <c r="D8" s="36">
-        <v>0.59740300000000002</v>
-      </c>
-      <c r="F8" s="33"/>
+      <c r="C8" s="32">
+        <v>0.2959</v>
+      </c>
+      <c r="D8" s="33">
+        <v>1</v>
+      </c>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="C9" s="35">
-        <v>2.6579999999999999</v>
-      </c>
-      <c r="D9" s="36">
-        <v>1.7982000000000001E-2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F9" s="33"/>
+      <c r="C9" s="32">
+        <v>0.72109999999999996</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0.92407600000000001</v>
+      </c>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
@@ -1562,115 +1610,142 @@
       <c r="D10" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="G10" s="33"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="34" t="s">
         <v>215</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C11" s="35">
-        <v>7.3773</v>
-      </c>
-      <c r="D11" s="36">
-        <v>2.9970000000000001E-3</v>
+      <c r="C11" s="32">
+        <v>12.8421</v>
+      </c>
+      <c r="D11" s="33">
+        <v>9.990000000000001E-4</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G11" s="33"/>
+        <v>203</v>
+      </c>
+      <c r="G11" s="31"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="31"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C12" s="35">
-        <v>2.8281999999999998</v>
-      </c>
-      <c r="D12" s="36">
-        <v>4.7952000000000002E-2</v>
+      <c r="C12" s="32">
+        <v>5.8544999999999998</v>
+      </c>
+      <c r="D12" s="33">
+        <v>8.9910000000000007E-3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G12" s="33"/>
+        <v>209</v>
+      </c>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="31"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="C13" s="35">
-        <v>80.863799999999998</v>
-      </c>
-      <c r="D13" s="36">
+      <c r="C13" s="32">
+        <v>36.661099999999998</v>
+      </c>
+      <c r="D13" s="33">
         <v>9.990000000000001E-4</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="G13" s="33"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="C14" s="35">
-        <v>2.1074999999999999</v>
-      </c>
-      <c r="D14" s="36">
-        <v>8.1918000000000005E-2</v>
-      </c>
-      <c r="G14" s="33"/>
+      <c r="C14" s="32">
+        <v>2.7393000000000001</v>
+      </c>
+      <c r="D14" s="33">
+        <v>5.3946000000000001E-2</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="31"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="C15" s="35">
-        <v>0.69879999999999998</v>
-      </c>
-      <c r="D15" s="36">
-        <v>0.514486</v>
-      </c>
-      <c r="G15" s="33"/>
+      <c r="C15" s="32">
+        <v>2.0301</v>
+      </c>
+      <c r="D15" s="33">
+        <v>2.0979000000000001E-2</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="31"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="C16" s="35">
-        <v>0.96179999999999999</v>
-      </c>
-      <c r="D16" s="36">
-        <v>0.36363600000000001</v>
-      </c>
-      <c r="G16" s="33"/>
+      <c r="C16" s="32">
+        <v>0.37530000000000002</v>
+      </c>
+      <c r="D16" s="33">
+        <v>0.98901099999999997</v>
+      </c>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="31"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="C17" s="35">
-        <v>1.0163</v>
-      </c>
-      <c r="D17" s="36">
-        <v>0.34565400000000002</v>
-      </c>
-      <c r="G17" s="33"/>
+      <c r="C17" s="32">
+        <v>0.4239</v>
+      </c>
+      <c r="D17" s="33">
+        <v>0.98101899999999997</v>
+      </c>
+      <c r="G17" s="31"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="36"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="36"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="36"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="36"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="36"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="36"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="A11:A17"/>
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1947,7 +2022,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="31">
+      <c r="A2" s="34">
         <v>1</v>
       </c>
       <c r="B2" s="10">
@@ -1971,7 +2046,7 @@
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="31"/>
+      <c r="A3" s="34"/>
       <c r="B3" s="10">
         <v>2</v>
       </c>
@@ -2001,7 +2076,7 @@
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="10">
         <v>3</v>
       </c>
@@ -2027,7 +2102,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="10">
         <v>4</v>
       </c>
@@ -2051,7 +2126,7 @@
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="10">
         <v>5</v>
       </c>
@@ -2073,7 +2148,7 @@
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="10">
         <v>6</v>
       </c>
@@ -2095,7 +2170,7 @@
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="31">
+      <c r="A8" s="34">
         <v>2</v>
       </c>
       <c r="B8" s="10">
@@ -2121,7 +2196,7 @@
       <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="10">
         <v>8</v>
       </c>
@@ -2145,7 +2220,7 @@
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="31"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="10">
         <v>9</v>
       </c>
@@ -2175,7 +2250,7 @@
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="10">
         <v>10</v>
       </c>
@@ -2199,7 +2274,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="31"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="10">
         <v>11</v>
       </c>
@@ -2223,7 +2298,7 @@
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="31"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="10">
         <v>12</v>
       </c>
@@ -2245,7 +2320,7 @@
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="10">
         <v>13</v>
       </c>
@@ -2267,7 +2342,7 @@
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="31">
+      <c r="A15" s="34">
         <v>3</v>
       </c>
       <c r="B15" s="10">
@@ -2291,7 +2366,7 @@
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="31"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="10">
         <v>15</v>
       </c>
@@ -2317,7 +2392,7 @@
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="31"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="10">
         <v>16</v>
       </c>
@@ -2347,7 +2422,7 @@
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="31"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="10">
         <v>17</v>
       </c>
@@ -2371,7 +2446,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="31"/>
+      <c r="A19" s="34"/>
       <c r="B19" s="10">
         <v>18</v>
       </c>
@@ -2393,7 +2468,7 @@
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="31"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="10">
         <v>19</v>
       </c>
@@ -2419,7 +2494,7 @@
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="10">
         <v>20</v>
       </c>
@@ -2441,7 +2516,7 @@
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="31">
+      <c r="A22" s="34">
         <v>4</v>
       </c>
       <c r="B22" s="10">
@@ -2465,7 +2540,7 @@
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="31"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="10">
         <v>22</v>
       </c>
@@ -2489,7 +2564,7 @@
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="31"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="10">
         <v>23</v>
       </c>
@@ -2521,7 +2596,7 @@
       <c r="L24" s="3"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="31"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="10">
         <v>24</v>
       </c>
@@ -2545,7 +2620,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="31"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="10">
         <v>25</v>
       </c>
@@ -2567,7 +2642,7 @@
       <c r="L26" s="3"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="31"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="10">
         <v>26</v>
       </c>
@@ -2589,7 +2664,7 @@
       <c r="L27" s="3"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="31"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="10">
         <v>27</v>
       </c>
@@ -2613,7 +2688,7 @@
       <c r="L28" s="3"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="31">
+      <c r="A29" s="34">
         <v>5</v>
       </c>
       <c r="B29" s="10">
@@ -2637,7 +2712,7 @@
       <c r="L29" s="3"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="31"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="10">
         <v>29</v>
       </c>
@@ -2663,7 +2738,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="31"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="10">
         <v>30</v>
       </c>
@@ -2693,7 +2768,7 @@
       <c r="L31" s="3"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="31"/>
+      <c r="A32" s="34"/>
       <c r="B32" s="10">
         <v>31</v>
       </c>
@@ -2717,7 +2792,7 @@
       <c r="L32" s="3"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="31"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="10">
         <v>32</v>
       </c>
@@ -2739,7 +2814,7 @@
       <c r="L33" s="3"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="31"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="10">
         <v>33</v>
       </c>
@@ -2761,7 +2836,7 @@
       <c r="L34" s="3"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="31"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="10">
         <v>34</v>
       </c>
@@ -2783,7 +2858,7 @@
       <c r="L35" s="3"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="31">
+      <c r="A36" s="34">
         <v>6</v>
       </c>
       <c r="B36" s="10">
@@ -2809,7 +2884,7 @@
       <c r="L36" s="3"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="31"/>
+      <c r="A37" s="34"/>
       <c r="B37" s="10">
         <v>36</v>
       </c>
@@ -2833,7 +2908,7 @@
       <c r="L37" s="3"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="31"/>
+      <c r="A38" s="34"/>
       <c r="B38" s="10">
         <v>37</v>
       </c>
@@ -2863,7 +2938,7 @@
       <c r="L38" s="3"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="31"/>
+      <c r="A39" s="34"/>
       <c r="B39" s="10">
         <v>38</v>
       </c>
@@ -2887,7 +2962,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="31"/>
+      <c r="A40" s="34"/>
       <c r="B40" s="10">
         <v>39</v>
       </c>
@@ -2913,7 +2988,7 @@
       <c r="L40" s="3"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="31"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="10">
         <v>40</v>
       </c>
@@ -2935,7 +3010,7 @@
       <c r="L41" s="3"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="31"/>
+      <c r="A42" s="34"/>
       <c r="B42" s="10">
         <v>41</v>
       </c>
@@ -2989,20 +3064,20 @@
     <row r="1" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
     </row>
     <row r="2" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -3315,20 +3390,20 @@
     <row r="9" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
     </row>
     <row r="10" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
@@ -3597,20 +3672,20 @@
     <row r="16" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
     </row>
     <row r="17" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -3976,14 +4051,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" style="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="18" bestFit="1" customWidth="1"/>

</xml_diff>